<commit_message>
added exceptions / main and added unit tests modified ClinicalTextDocument's constructor to accept none or ' '  without parsing text
</commit_message>
<xml_diff>
--- a/sample_annotations.xlsx
+++ b/sample_annotations.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\LocalAdmin\Downloads\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="420" yWindow="588" windowWidth="18564" windowHeight="6096"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="3144" windowHeight="384"/>
   </bookViews>
   <sheets>
     <sheet name="PBM_Review_Summary" sheetId="1" r:id="rId1"/>
@@ -17,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="29">
   <si>
     <t>File Name with extension</t>
   </si>
@@ -98,6 +103,12 @@
   </si>
   <si>
     <t>historical</t>
+  </si>
+  <si>
+    <t>[123414,150169]</t>
+  </si>
+  <si>
+    <t>( 1234,15069)</t>
   </si>
 </sst>
 </file>
@@ -133,8 +144,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -144,6 +156,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -192,7 +207,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -227,7 +242,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -436,10 +451,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K6"/>
+  <dimension ref="A1:K7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A8" sqref="A8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D9" sqref="D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -447,7 +462,7 @@
     <col min="1" max="1" width="54.33203125" customWidth="1"/>
     <col min="2" max="2" width="39" customWidth="1"/>
     <col min="3" max="3" width="52.33203125" customWidth="1"/>
-    <col min="4" max="4" width="20.21875" customWidth="1"/>
+    <col min="4" max="4" width="20.21875" style="1" customWidth="1"/>
     <col min="5" max="5" width="21.21875" customWidth="1"/>
     <col min="6" max="6" width="20.6640625" customWidth="1"/>
   </cols>
@@ -462,7 +477,7 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
       <c r="E1" t="s">
@@ -479,7 +494,7 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" t="s">
+      <c r="D2" s="1" t="s">
         <v>12</v>
       </c>
       <c r="E2" t="s">
@@ -496,7 +511,7 @@
       <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="D3" t="s">
+      <c r="D3" s="1" t="s">
         <v>9</v>
       </c>
       <c r="E3" t="s">
@@ -513,8 +528,8 @@
       <c r="C4" t="s">
         <v>13</v>
       </c>
-      <c r="D4" t="s">
-        <v>14</v>
+      <c r="D4" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="E4" t="s">
         <v>15</v>
@@ -548,7 +563,7 @@
       <c r="C5" t="s">
         <v>24</v>
       </c>
-      <c r="D5" t="s">
+      <c r="D5" s="1" t="s">
         <v>14</v>
       </c>
       <c r="E5" t="s">
@@ -578,8 +593,14 @@
         <v>22</v>
       </c>
     </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.3">
+      <c r="D7" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
   </sheetData>
   <autoFilter ref="A1:K5"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>